<commit_message>
Minor R and code mapping updates
</commit_message>
<xml_diff>
--- a/Korean_Codes/DGRSLT_TP_CD.xlsx
+++ b/Korean_Codes/DGRSLT_TP_CD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Korea/opendata4covid19/Korean_Codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6F225F-6D77-EE45-BFD8-2C2D50FDC244}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7B0AEA-4712-C247-92AF-F80E3AAA6385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="5680" windowWidth="27640" windowHeight="16940" xr2:uid="{0F47D111-F58C-B646-BB10-4799C9C0DFD1}"/>
+    <workbookView xWindow="21780" yWindow="5380" windowWidth="27640" windowHeight="16940" xr2:uid="{0F47D111-F58C-B646-BB10-4799C9C0DFD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>DGRSLT_TP_CD</t>
   </si>
@@ -41,25 +41,28 @@
     <t>OUTCOME</t>
   </si>
   <si>
-    <t>continued</t>
-  </si>
-  <si>
-    <t>transfer</t>
-  </si>
-  <si>
-    <t>returned</t>
-  </si>
-  <si>
-    <t>dead</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>previous</t>
-  </si>
-  <si>
     <t>$</t>
+  </si>
+  <si>
+    <t>Continued</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>Discharge</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -450,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -458,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -466,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -474,7 +477,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -482,7 +485,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -490,15 +493,15 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>